<commit_message>
several changes made. Impossible to track them
</commit_message>
<xml_diff>
--- a/01-raw-data/IMF data/ppp rate.xlsx
+++ b/01-raw-data/IMF data/ppp rate.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ee9ef301486063b/Documentos/GitHub/Large-Devaluations-and-CO2/01-raw-data/IMF data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_AD4D2F04E46CFB4ACB3E20F30D57FB54683EDF23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83E45CE-A866-4423-BACB-A0865511B991}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_AD4D2F04E46CFB4ACB3E20F30D57FB54683EDF23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B10B5BCF-5124-4CBB-AF57-4491C53E6058}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPPEX" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PPPEX!$A$1:$AY$197</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="199">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -955,10 +958,10 @@
   <dimension ref="A1:AY199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A198" sqref="A198"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2495,11 +2498,11 @@
       <c r="K9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>1</v>
+      <c r="L9" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="N9" s="1">
         <v>5.2999999999999999E-2</v>
@@ -3115,14 +3118,14 @@
       <c r="K13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>1</v>
+      <c r="L13" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1E-3</v>
       </c>
       <c r="N13" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="O13" s="1">
         <v>1E-3</v>
@@ -3890,26 +3893,26 @@
       <c r="K18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>1</v>
+      <c r="L18" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1E-3</v>
       </c>
       <c r="N18" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="O18" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="Q18" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="R18" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="S18" s="1">
         <v>1E-3</v>
@@ -4820,17 +4823,17 @@
       <c r="K24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>1</v>
+      <c r="L24" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0.48099999999999998</v>
       </c>
       <c r="P24" s="1">
         <v>0.48099999999999998</v>
@@ -5131,10 +5134,10 @@
         <v>0</v>
       </c>
       <c r="L26" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="M26" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="N26" s="1">
         <v>1E-3</v>
@@ -7456,16 +7459,16 @@
         <v>0</v>
       </c>
       <c r="L41" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="M41" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="N41" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O41" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="P41" s="1">
         <v>1.2999999999999999E-2</v>
@@ -7920,11 +7923,11 @@
       <c r="K44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>1</v>
+      <c r="L44" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N44" s="1">
         <v>1.0999999999999999E-2</v>
@@ -8230,20 +8233,20 @@
       <c r="K46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>1</v>
+      <c r="L46" s="1">
+        <v>10.91</v>
+      </c>
+      <c r="M46" s="1">
+        <v>10.91</v>
+      </c>
+      <c r="N46" s="1">
+        <v>10.91</v>
+      </c>
+      <c r="O46" s="1">
+        <v>10.91</v>
+      </c>
+      <c r="P46" s="1">
+        <v>10.91</v>
       </c>
       <c r="Q46" s="1">
         <v>10.91</v>
@@ -9780,11 +9783,11 @@
       <c r="K56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>1</v>
+      <c r="L56" s="1">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="M56" s="1">
+        <v>1.0009999999999999</v>
       </c>
       <c r="N56" s="1">
         <v>1.0009999999999999</v>
@@ -9935,14 +9938,14 @@
       <c r="K57" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N57" s="1" t="s">
-        <v>1</v>
+      <c r="L57" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="M57" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="N57" s="1">
+        <v>0.13500000000000001</v>
       </c>
       <c r="O57" s="1">
         <v>0.13500000000000001</v>
@@ -11176,13 +11179,13 @@
         <v>1</v>
       </c>
       <c r="L65" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="M65" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="N65" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="O65" s="1">
         <v>1E-3</v>
@@ -13810,29 +13813,29 @@
       <c r="K82" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S82" s="1" t="s">
-        <v>1</v>
+      <c r="L82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="M82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="N82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="O82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="P82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="R82" s="1">
+        <v>213.999</v>
+      </c>
+      <c r="S82" s="1">
+        <v>213.999</v>
       </c>
       <c r="T82" s="1">
         <v>213.999</v>
@@ -14895,11 +14898,11 @@
       <c r="K89" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L89" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>1</v>
+      <c r="L89" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M89" s="1">
+        <v>0.02</v>
       </c>
       <c r="N89" s="1">
         <v>0.02</v>
@@ -16135,11 +16138,11 @@
       <c r="K97" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L97" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M97" s="1" t="s">
-        <v>1</v>
+      <c r="L97" s="1">
+        <v>0.111</v>
+      </c>
+      <c r="M97" s="1">
+        <v>0.111</v>
       </c>
       <c r="N97" s="1">
         <v>0.111</v>
@@ -16910,20 +16913,20 @@
       <c r="K102" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L102" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M102" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N102" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O102" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P102" s="1" t="s">
-        <v>1</v>
+      <c r="L102" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="M102" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="N102" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="O102" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="P102" s="1">
+        <v>0.312</v>
       </c>
       <c r="Q102" s="1">
         <v>0.312</v>
@@ -19080,8 +19083,8 @@
       <c r="K116" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L116" s="1" t="s">
-        <v>1</v>
+      <c r="L116" s="1">
+        <v>1E-3</v>
       </c>
       <c r="M116" s="1">
         <v>1E-3</v>
@@ -19855,29 +19858,29 @@
       <c r="K121" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S121" s="1" t="s">
-        <v>1</v>
+      <c r="L121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="M121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="N121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="O121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="P121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="Q121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="R121" s="1">
+        <v>44.457000000000001</v>
+      </c>
+      <c r="S121" s="1">
+        <v>44.457000000000001</v>
       </c>
       <c r="T121" s="1">
         <v>44.457000000000001</v>
@@ -21250,11 +21253,11 @@
       <c r="K130" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L130" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M130" s="1" t="s">
-        <v>1</v>
+      <c r="L130" s="1">
+        <v>1.0720000000000001</v>
+      </c>
+      <c r="M130" s="1">
+        <v>1.0720000000000001</v>
       </c>
       <c r="N130" s="1">
         <v>1.0720000000000001</v>
@@ -23421,7 +23424,7 @@
         <v>0</v>
       </c>
       <c r="L144" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="M144" s="1">
         <v>1E-3</v>
@@ -23576,7 +23579,7 @@
         <v>1</v>
       </c>
       <c r="L145" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="M145" s="1">
         <v>1E-3</v>
@@ -24505,26 +24508,26 @@
       <c r="K151" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R151" s="1" t="s">
-        <v>1</v>
+      <c r="L151" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="M151" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="N151" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="O151" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="P151" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="Q151" s="1">
+        <v>0.747</v>
+      </c>
+      <c r="R151" s="1">
+        <v>0.747</v>
       </c>
       <c r="S151" s="1">
         <v>0.747</v>
@@ -24970,26 +24973,26 @@
       <c r="K154" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R154" s="1" t="s">
-        <v>1</v>
+      <c r="L154" s="1">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="M154" s="1">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="N154" s="1">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="O154" s="1">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="P154" s="1">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="Q154" s="1">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="R154" s="1">
+        <v>3.2290000000000001</v>
       </c>
       <c r="S154" s="1">
         <v>3.2290000000000001</v>
@@ -25745,11 +25748,11 @@
       <c r="K159" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L159" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M159" s="1" t="s">
-        <v>1</v>
+      <c r="L159" s="1">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="M159" s="1">
+        <v>0.28799999999999998</v>
       </c>
       <c r="N159" s="1">
         <v>0.28799999999999998</v>
@@ -27915,14 +27918,14 @@
       <c r="K173" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L173" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M173" s="1" t="s">
-        <v>1</v>
+      <c r="L173" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M173" s="1">
+        <v>1E-3</v>
       </c>
       <c r="N173" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="O173" s="1">
         <v>1E-3</v>
@@ -29155,17 +29158,17 @@
       <c r="K181" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L181" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M181" s="1" t="s">
-        <v>1</v>
+      <c r="L181" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="M181" s="1">
+        <v>2E-3</v>
       </c>
       <c r="N181" s="1">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="O181" s="1">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="P181" s="1">
         <v>2E-3</v>
@@ -29775,14 +29778,14 @@
       <c r="K185" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L185" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M185" s="1" t="s">
-        <v>1</v>
+      <c r="L185" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M185" s="1">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N185" s="1">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O185" s="1">
         <v>5.0000000000000001E-3</v>
@@ -30550,8 +30553,8 @@
       <c r="K190" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L190" s="1" t="s">
-        <v>1</v>
+      <c r="L190" s="1">
+        <v>1E-3</v>
       </c>
       <c r="M190" s="1">
         <v>1E-3</v>
@@ -31635,29 +31638,29 @@
       <c r="K197" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S197" s="1" t="s">
-        <v>1</v>
+      <c r="L197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="M197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="N197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="O197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="P197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="Q197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="R197" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="S197" s="1">
+        <v>0.42199999999999999</v>
       </c>
       <c r="T197" s="1">
         <v>0.42199999999999999</v>

</xml_diff>